<commit_message>
Corrected a test result. Added the image with the tests
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -77,6 +77,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -98,6 +99,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -175,7 +177,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>